<commit_message>
Update the 'Example_Report_1.xlsx' test file as necessary for changes in the main branch
</commit_message>
<xml_diff>
--- a/tests/test_files/reports/Example_Report_1.xlsx
+++ b/tests/test_files/reports/Example_Report_1.xlsx
@@ -10,17 +10,23 @@
     <sheet name="individual_report_1" sheetId="1" r:id="rId1"/>
     <sheet name="group_report_1" sheetId="2" r:id="rId2"/>
     <sheet name="overall_report_1" sheetId="3" r:id="rId3"/>
+    <sheet name="individual_report_2" sheetId="4" r:id="rId4"/>
+    <sheet name="group_report_2" sheetId="5" r:id="rId5"/>
+    <sheet name="overall_report_2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="54">
   <si>
     <t>Student Id</t>
   </si>
   <si>
+    <t>Disliked Students</t>
+  </si>
+  <si>
     <t>Meets Dislike Requirement</t>
   </si>
   <si>
@@ -54,6 +60,27 @@
     <t>Group Id</t>
   </si>
   <si>
+    <t>mmuster3</t>
+  </si>
+  <si>
+    <t>jdoe2</t>
+  </si>
+  <si>
+    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM;thursday @ 3:00 PM - 6:00 PM;thursday @ 6:00 PM - 9:00 PM;friday @ 9:00 PM - 12:00 PM</t>
+  </si>
+  <si>
+    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM</t>
+  </si>
+  <si>
+    <t>bwillia5;jsmith1</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>bwillia5</t>
   </si>
   <si>
@@ -63,42 +90,24 @@
     <t>monday @ 0:00 AM - 3:00 AM;tuesday @ 0:00 AM - 3:00 AM;wednesday @ 0:00 AM - 3:00 AM;thursday @ 0:00 AM - 3:00 AM;friday @ 0:00 AM - 3:00 AM;saturday @ 0:00 AM - 3:00 AM;sunday @ 0:00 AM - 3:00 AM;monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 AM - 6:00 AM;thursday @ 3:00 AM - 6:00 AM;friday @ 3:00 AM - 6:00 AM;saturday @ 3:00 AM - 6:00 AM;sunday @ 3:00 AM - 6:00 AM;monday @ 6:00 AM - 9:00 AM;tuesday @ 6:00 AM - 9:00 AM;wednesday @ 6:00 AM - 9:00 AM;thursday @ 6:00 AM - 9:00 AM;friday @ 6:00 AM - 9:00 AM;saturday @ 6:00 AM - 9:00 AM;sunday @ 6:00 AM - 9:00 AM;monday @ 9:00 AM - 12:00 PM;tuesday @ 9:00 AM - 12:00 PM;wednesday @ 9:00 AM - 12:00 PM;thursday @ 9:00 AM - 12:00 PM;friday @ 9:00 AM - 12:00 PM;saturday @ 9:00 AM - 12:00 PM;sunday @ 9:00 AM - 12:00 PM;monday @ 12:00 PM - 3:00 PM;tuesday @ 12:00 PM - 3:00 PM;wednesday @ 12:00 PM - 3:00 PM;thursday @ 12:00 PM - 3:00 PM;friday @ 12:00 PM - 3:00 PM;saturday @ 12:00 PM - 3:00 PM;sunday @ 12:00 PM - 3:00 PM;monday @ 3:00 PM - 6:00 PM;tuesday @ 3:00 PM - 6:00 PM;wednesday @ 3:00 PM - 6:00 PM;thursday @ 3:00 PM - 6:00 PM;friday @ 3:00 PM - 6:00 PM;saturday @ 3:00 PM - 6:00 PM;sunday @ 3:00 PM - 6:00 PM;monday @ 6:00 PM - 9:00 PM;tuesday @ 6:00 PM - 9:00 PM;wednesday @ 6:00 PM - 9:00 PM;thursday @ 6:00 PM - 9:00 PM;friday @ 6:00 PM - 9:00 PM;saturday @ 6:00 PM - 9:00 PM;sunday @ 6:00 PM - 9:00 PM;monday @ 9:00 PM - 12:00 PM;tuesday @ 9:00 PM - 12:00 PM;wednesday @ 9:00 PM - 12:00 PM;thursday @ 9:00 PM - 12:00 PM;friday @ 9:00 PM - 12:00 PM;saturday @ 9:00 PM - 12:00 PM;sunday @ 9:00 PM - 12:00 PM</t>
   </si>
   <si>
-    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>False</t>
   </si>
   <si>
     <t>jsmith1</t>
   </si>
   <si>
-    <t>mmuster3</t>
+    <t>jschmo4;mmuster3</t>
   </si>
   <si>
     <t>sunday @ 0:00 AM - 3:00 AM;thursday @ 0:00 AM - 3:00 AM;friday @ 0:00 AM - 3:00 AM;monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 PM - 6:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
   </si>
   <si>
-    <t>jdoe2</t>
-  </si>
-  <si>
-    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM;thursday @ 3:00 PM - 6:00 PM;thursday @ 6:00 PM - 9:00 PM;friday @ 9:00 PM - 12:00 PM</t>
-  </si>
-  <si>
-    <t>bwillia5;jsmith1</t>
+    <t>jschmo4</t>
   </si>
   <si>
     <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 12:00 PM - 3:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
   </si>
   <si>
-    <t>jschmo4;mmuster3</t>
-  </si>
-  <si>
-    <t>jschmo4</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -154,6 +163,24 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>group_1</t>
+  </si>
+  <si>
+    <t>group_2</t>
+  </si>
+  <si>
+    <t>jsmith1/jdoe2</t>
+  </si>
+  <si>
+    <t>jdoe2/jsmith1</t>
+  </si>
+  <si>
+    <t>mmuster3/bwillia5</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -485,13 +512,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,168 +555,180 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -707,45 +746,45 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -754,25 +793,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I2">
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -783,7 +822,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -795,13 +834,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -828,48 +867,454 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2">
         <v>-20.6875</v>
       </c>
       <c r="G2">
         <v>10.451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>-20.895</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0.1125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2">
+        <v>-20.7825</v>
+      </c>
+      <c r="G2">
+        <v>10.504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Load the survey data from the temp csv and then delete it (the temp csv)
* Update the existing tests as necessary for the changes made
</commit_message>
<xml_diff>
--- a/tests/test_files/reports/Example_Report_1.xlsx
+++ b/tests/test_files/reports/Example_Report_1.xlsx
@@ -13,13 +13,14 @@
     <sheet name="individual_report_2" sheetId="4" r:id="rId4"/>
     <sheet name="group_report_2" sheetId="5" r:id="rId5"/>
     <sheet name="overall_report_2" sheetId="6" r:id="rId6"/>
+    <sheet name="survey_data" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="107">
   <si>
     <t>Student Id</t>
   </si>
@@ -60,25 +61,34 @@
     <t>Group Id</t>
   </si>
   <si>
+    <t>jsmith1</t>
+  </si>
+  <si>
+    <t>mmuster3;jschmo4</t>
+  </si>
+  <si>
     <t>mmuster3</t>
   </si>
   <si>
+    <t>sunday @ 0:00 AM - 3:00 AM;thursday @ 0:00 AM - 3:00 AM;friday @ 0:00 AM - 3:00 AM;monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 PM - 6:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
+  </si>
+  <si>
+    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM</t>
+  </si>
+  <si>
     <t>jdoe2</t>
   </si>
   <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM;thursday @ 3:00 PM - 6:00 PM;thursday @ 6:00 PM - 9:00 PM;friday @ 9:00 PM - 12:00 PM</t>
   </si>
   <si>
-    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM</t>
-  </si>
-  <si>
-    <t>bwillia5;jsmith1</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>jsmith1;bwillia5</t>
   </si>
   <si>
     <t>bwillia5</t>
@@ -93,21 +103,12 @@
     <t>False</t>
   </si>
   <si>
-    <t>jsmith1</t>
-  </si>
-  <si>
-    <t>jschmo4;mmuster3</t>
-  </si>
-  <si>
-    <t>sunday @ 0:00 AM - 3:00 AM;thursday @ 0:00 AM - 3:00 AM;friday @ 0:00 AM - 3:00 AM;monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 PM - 6:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
+    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 12:00 PM - 3:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
   </si>
   <si>
     <t>jschmo4</t>
   </si>
   <si>
-    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 12:00 PM - 3:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -129,7 +130,7 @@
     <t>Score</t>
   </si>
   <si>
-    <t>mmuster3/bwillia5;mmuster3/jsmith1</t>
+    <t>mmuster3/jsmith1;mmuster3/bwillia5</t>
   </si>
   <si>
     <t>jsmith1/mmuster3</t>
@@ -181,6 +182,165 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Please select your ASURITE ID</t>
+  </si>
+  <si>
+    <t>Please enter your Github username (NOT your email address)</t>
+  </si>
+  <si>
+    <t>Email address for us to invite you to the Taiga scrumboard</t>
+  </si>
+  <si>
+    <t>In what time zone do you live or will you be during the session? Please use UTC so we can match it easier.</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [0:00 AM - 3:00 AM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 AM - 6:00 AM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 AM - 9:00 AM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 AM - 12:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [12:00 PM - 3:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 PM - 6:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 PM - 9:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 PM - 12:00 PM]</t>
+  </si>
+  <si>
+    <t>How well would you say you know GitHub? (1 not at all, 5 worked with it a lot - know how to merge, resolve conflicts, etc.) You are not expected to know GitHub well yet, so please be honest. It will not be used for grading what you put here but I want to try to have one student knowing GitHub in each team to make things easier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you know Scrum already? (1 just heard about it, 5 know it well (process, roles). You are not expected to know Scrum yet, so please be honest. It will not be used for grading what you put here. </t>
+  </si>
+  <si>
+    <t>Preferred team member 1</t>
+  </si>
+  <si>
+    <t>Preferred team member 2</t>
+  </si>
+  <si>
+    <t>Preferred team member 3</t>
+  </si>
+  <si>
+    <t>Preferred team member 4</t>
+  </si>
+  <si>
+    <t>Preferred team member 5</t>
+  </si>
+  <si>
+    <t>Non-preferred student 1</t>
+  </si>
+  <si>
+    <t>Non-preferred student 2</t>
+  </si>
+  <si>
+    <t>Non-preferred student 3</t>
+  </si>
+  <si>
+    <t>2022/10/17 6:31:58 PM EST</t>
+  </si>
+  <si>
+    <t>jsmith1@asu.edu</t>
+  </si>
+  <si>
+    <t>jsmith_1</t>
+  </si>
+  <si>
+    <t>johnsmith@gmail.com</t>
+  </si>
+  <si>
+    <t>UTC +1</t>
+  </si>
+  <si>
+    <t>Sunday;Thursday;Friday</t>
+  </si>
+  <si>
+    <t>Monday;Tuesday</t>
+  </si>
+  <si>
+    <t>Tuesday;Wednesday</t>
+  </si>
+  <si>
+    <t>jdoe2 - Jane Doe</t>
+  </si>
+  <si>
+    <t>mmuster3 - Max Mustermann</t>
+  </si>
+  <si>
+    <t>jschmo4 - Joe Schmo</t>
+  </si>
+  <si>
+    <t>2022/10/17 6:33:27 PM EST</t>
+  </si>
+  <si>
+    <t>jdoe2@asu.edu</t>
+  </si>
+  <si>
+    <t>jdoe_2</t>
+  </si>
+  <si>
+    <t>janedoe@gmail.com</t>
+  </si>
+  <si>
+    <t>UTC +2</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>jsmith1 - John Smith</t>
+  </si>
+  <si>
+    <t>bwillia5 - Billy Williams</t>
+  </si>
+  <si>
+    <t>2022/10/17 6:34:15 PM EST</t>
+  </si>
+  <si>
+    <t>mmuster3@asu.edu</t>
+  </si>
+  <si>
+    <t>mmuster_3</t>
+  </si>
+  <si>
+    <t>maxmustermann@gmail.com</t>
+  </si>
+  <si>
+    <t>UTC +3</t>
+  </si>
+  <si>
+    <t>Wednesday;Thursday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -567,127 +727,136 @@
         <v>14</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
         <v>29</v>
@@ -695,37 +864,28 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
         <v>27</v>
       </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
         <v>29</v>
@@ -784,7 +944,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -793,13 +953,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -834,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -893,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -967,37 +1127,37 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
         <v>48</v>
@@ -1005,37 +1165,37 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s">
         <v>48</v>
@@ -1043,37 +1203,37 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
         <v>49</v>
@@ -1081,28 +1241,28 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
         <v>49</v>
@@ -1110,28 +1270,28 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
         <v>49</v>
@@ -1199,13 +1359,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -1240,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1299,7 +1459,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -1315,6 +1475,241 @@
       </c>
       <c r="G2">
         <v>10.504</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>86</v>
+      </c>
+      <c r="V2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O3" t="s">
+        <v>96</v>
+      </c>
+      <c r="P3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>87</v>
+      </c>
+      <c r="R3" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>97</v>
+      </c>
+      <c r="R4" t="s">
+        <v>98</v>
+      </c>
+      <c r="V4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="C6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TSK#199: Reading (loading) raw survey data from a report (#83)
* Create a 'temp' csv file from the 'survey_data' sheet of the report

* * Load the survey data from the temp csv and then delete it (the temp csv)

* Update the existing tests as necessary for the changes made

* Write and read the report's survey data via an IO buffer instead of a temp CSV file, per a review comment recommendation
</commit_message>
<xml_diff>
--- a/tests/test_files/reports/Example_Report_1.xlsx
+++ b/tests/test_files/reports/Example_Report_1.xlsx
@@ -13,13 +13,14 @@
     <sheet name="individual_report_2" sheetId="4" r:id="rId4"/>
     <sheet name="group_report_2" sheetId="5" r:id="rId5"/>
     <sheet name="overall_report_2" sheetId="6" r:id="rId6"/>
+    <sheet name="survey_data" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="107">
   <si>
     <t>Student Id</t>
   </si>
@@ -60,25 +61,34 @@
     <t>Group Id</t>
   </si>
   <si>
+    <t>jsmith1</t>
+  </si>
+  <si>
+    <t>mmuster3;jschmo4</t>
+  </si>
+  <si>
     <t>mmuster3</t>
   </si>
   <si>
+    <t>sunday @ 0:00 AM - 3:00 AM;thursday @ 0:00 AM - 3:00 AM;friday @ 0:00 AM - 3:00 AM;monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 PM - 6:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
+  </si>
+  <si>
+    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM</t>
+  </si>
+  <si>
     <t>jdoe2</t>
   </si>
   <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM;thursday @ 3:00 PM - 6:00 PM;thursday @ 6:00 PM - 9:00 PM;friday @ 9:00 PM - 12:00 PM</t>
   </si>
   <si>
-    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM</t>
-  </si>
-  <si>
-    <t>bwillia5;jsmith1</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>jsmith1;bwillia5</t>
   </si>
   <si>
     <t>bwillia5</t>
@@ -93,21 +103,12 @@
     <t>False</t>
   </si>
   <si>
-    <t>jsmith1</t>
-  </si>
-  <si>
-    <t>jschmo4;mmuster3</t>
-  </si>
-  <si>
-    <t>sunday @ 0:00 AM - 3:00 AM;thursday @ 0:00 AM - 3:00 AM;friday @ 0:00 AM - 3:00 AM;monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 PM - 6:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
+    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 12:00 PM - 3:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
   </si>
   <si>
     <t>jschmo4</t>
   </si>
   <si>
-    <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;tuesday @ 12:00 PM - 3:00 PM;wednesday @ 3:00 PM - 6:00 PM</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -129,7 +130,7 @@
     <t>Score</t>
   </si>
   <si>
-    <t>mmuster3/bwillia5;mmuster3/jsmith1</t>
+    <t>mmuster3/jsmith1;mmuster3/bwillia5</t>
   </si>
   <si>
     <t>jsmith1/mmuster3</t>
@@ -181,6 +182,165 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Please select your ASURITE ID</t>
+  </si>
+  <si>
+    <t>Please enter your Github username (NOT your email address)</t>
+  </si>
+  <si>
+    <t>Email address for us to invite you to the Taiga scrumboard</t>
+  </si>
+  <si>
+    <t>In what time zone do you live or will you be during the session? Please use UTC so we can match it easier.</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [0:00 AM - 3:00 AM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 AM - 6:00 AM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 AM - 9:00 AM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 AM - 12:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [12:00 PM - 3:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 PM - 6:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 PM - 9:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 PM - 12:00 PM]</t>
+  </si>
+  <si>
+    <t>How well would you say you know GitHub? (1 not at all, 5 worked with it a lot - know how to merge, resolve conflicts, etc.) You are not expected to know GitHub well yet, so please be honest. It will not be used for grading what you put here but I want to try to have one student knowing GitHub in each team to make things easier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you know Scrum already? (1 just heard about it, 5 know it well (process, roles). You are not expected to know Scrum yet, so please be honest. It will not be used for grading what you put here. </t>
+  </si>
+  <si>
+    <t>Preferred team member 1</t>
+  </si>
+  <si>
+    <t>Preferred team member 2</t>
+  </si>
+  <si>
+    <t>Preferred team member 3</t>
+  </si>
+  <si>
+    <t>Preferred team member 4</t>
+  </si>
+  <si>
+    <t>Preferred team member 5</t>
+  </si>
+  <si>
+    <t>Non-preferred student 1</t>
+  </si>
+  <si>
+    <t>Non-preferred student 2</t>
+  </si>
+  <si>
+    <t>Non-preferred student 3</t>
+  </si>
+  <si>
+    <t>2022/10/17 6:31:58 PM EST</t>
+  </si>
+  <si>
+    <t>jsmith1@asu.edu</t>
+  </si>
+  <si>
+    <t>jsmith_1</t>
+  </si>
+  <si>
+    <t>johnsmith@gmail.com</t>
+  </si>
+  <si>
+    <t>UTC +1</t>
+  </si>
+  <si>
+    <t>Sunday;Thursday;Friday</t>
+  </si>
+  <si>
+    <t>Monday;Tuesday</t>
+  </si>
+  <si>
+    <t>Tuesday;Wednesday</t>
+  </si>
+  <si>
+    <t>jdoe2 - Jane Doe</t>
+  </si>
+  <si>
+    <t>mmuster3 - Max Mustermann</t>
+  </si>
+  <si>
+    <t>jschmo4 - Joe Schmo</t>
+  </si>
+  <si>
+    <t>2022/10/17 6:33:27 PM EST</t>
+  </si>
+  <si>
+    <t>jdoe2@asu.edu</t>
+  </si>
+  <si>
+    <t>jdoe_2</t>
+  </si>
+  <si>
+    <t>janedoe@gmail.com</t>
+  </si>
+  <si>
+    <t>UTC +2</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>jsmith1 - John Smith</t>
+  </si>
+  <si>
+    <t>bwillia5 - Billy Williams</t>
+  </si>
+  <si>
+    <t>2022/10/17 6:34:15 PM EST</t>
+  </si>
+  <si>
+    <t>mmuster3@asu.edu</t>
+  </si>
+  <si>
+    <t>mmuster_3</t>
+  </si>
+  <si>
+    <t>maxmustermann@gmail.com</t>
+  </si>
+  <si>
+    <t>UTC +3</t>
+  </si>
+  <si>
+    <t>Wednesday;Thursday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -567,127 +727,136 @@
         <v>14</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
         <v>29</v>
@@ -695,37 +864,28 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
         <v>27</v>
       </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
         <v>29</v>
@@ -784,7 +944,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -793,13 +953,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -834,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -893,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -967,37 +1127,37 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
         <v>48</v>
@@ -1005,37 +1165,37 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s">
         <v>48</v>
@@ -1043,37 +1203,37 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
         <v>49</v>
@@ -1081,28 +1241,28 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
         <v>49</v>
@@ -1110,28 +1270,28 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
         <v>49</v>
@@ -1199,13 +1359,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -1240,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1299,7 +1459,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -1315,6 +1475,241 @@
       </c>
       <c r="G2">
         <v>10.504</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>86</v>
+      </c>
+      <c r="V2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O3" t="s">
+        <v>96</v>
+      </c>
+      <c r="P3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>87</v>
+      </c>
+      <c r="R3" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>97</v>
+      </c>
+      <c r="R4" t="s">
+        <v>98</v>
+      </c>
+      <c r="V4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="C6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update as necessary after merging updates for Taiga task #200 (related to reading config data from the report) from main
</commit_message>
<xml_diff>
--- a/tests/test_files/reports/Example_Report_1.xlsx
+++ b/tests/test_files/reports/Example_Report_1.xlsx
@@ -13,14 +13,15 @@
     <sheet name="individual_report_2" sheetId="4" r:id="rId4"/>
     <sheet name="group_report_2" sheetId="5" r:id="rId5"/>
     <sheet name="overall_report_2" sheetId="6" r:id="rId6"/>
-    <sheet name="survey_data" sheetId="7" r:id="rId7"/>
+    <sheet name="config" sheetId="7" r:id="rId7"/>
+    <sheet name="survey_data" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="127">
   <si>
     <t>Student Id</t>
   </si>
@@ -88,7 +89,7 @@
     <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM;thursday @ 3:00 PM - 6:00 PM;thursday @ 6:00 PM - 9:00 PM;friday @ 9:00 PM - 12:00 PM</t>
   </si>
   <si>
-    <t>jsmith1;bwillia5</t>
+    <t>bwillia5;jsmith1</t>
   </si>
   <si>
     <t>bwillia5</t>
@@ -130,7 +131,7 @@
     <t>Score</t>
   </si>
   <si>
-    <t>mmuster3/jsmith1;mmuster3/bwillia5</t>
+    <t>mmuster3/bwillia5;mmuster3/jsmith1</t>
   </si>
   <si>
     <t>jsmith1/mmuster3</t>
@@ -184,76 +185,136 @@
     <t>7</t>
   </si>
   <si>
+    <t>class_name</t>
+  </si>
+  <si>
+    <t>target_group_size</t>
+  </si>
+  <si>
+    <t>target_plus_one_allowed</t>
+  </si>
+  <si>
+    <t>target_minus_one_allowed</t>
+  </si>
+  <si>
+    <t>grouping_passes</t>
+  </si>
+  <si>
+    <t>availability_values_delimiter</t>
+  </si>
+  <si>
+    <t>student_id_field_name</t>
+  </si>
+  <si>
+    <t>timezone_field_name</t>
+  </si>
+  <si>
+    <t>preferred_students_field_names</t>
+  </si>
+  <si>
+    <t>disliked_students_field_names</t>
+  </si>
+  <si>
+    <t>availability_field_names</t>
+  </si>
+  <si>
+    <t>show_preferred_students</t>
+  </si>
+  <si>
+    <t>show_disliked_students</t>
+  </si>
+  <si>
+    <t>show_availability_overlap</t>
+  </si>
+  <si>
+    <t>show_scores</t>
+  </si>
+  <si>
+    <t>output_student_name</t>
+  </si>
+  <si>
+    <t>output_student_email</t>
+  </si>
+  <si>
+    <t>output_student_login</t>
+  </si>
+  <si>
+    <t>SER401</t>
+  </si>
+  <si>
+    <t>;,</t>
+  </si>
+  <si>
+    <t>Please select your ASURITE ID</t>
+  </si>
+  <si>
+    <t>In what time zone do you live or will you be during the session? Please use UTC so we can match it easier.</t>
+  </si>
+  <si>
+    <t>Preferred team member 1</t>
+  </si>
+  <si>
+    <t>Non-preferred student 1</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [0:00 AM - 3:00 AM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 2</t>
+  </si>
+  <si>
+    <t>Non-preferred student 2</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 AM - 6:00 AM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 3</t>
+  </si>
+  <si>
+    <t>Non-preferred student 3</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 AM - 9:00 AM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 4</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 AM - 12:00 PM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 5</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [12:00 PM - 3:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 PM - 6:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 PM - 9:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 PM - 12:00 PM]</t>
+  </si>
+  <si>
     <t>Timestamp</t>
   </si>
   <si>
     <t>Username</t>
   </si>
   <si>
-    <t>Please select your ASURITE ID</t>
-  </si>
-  <si>
     <t>Please enter your Github username (NOT your email address)</t>
   </si>
   <si>
     <t>Email address for us to invite you to the Taiga scrumboard</t>
   </si>
   <si>
-    <t>In what time zone do you live or will you be during the session? Please use UTC so we can match it easier.</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [0:00 AM - 3:00 AM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 AM - 6:00 AM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 AM - 9:00 AM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 AM - 12:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [12:00 PM - 3:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 PM - 6:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 PM - 9:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 PM - 12:00 PM]</t>
-  </si>
-  <si>
     <t>How well would you say you know GitHub? (1 not at all, 5 worked with it a lot - know how to merge, resolve conflicts, etc.) You are not expected to know GitHub well yet, so please be honest. It will not be used for grading what you put here but I want to try to have one student knowing GitHub in each team to make things easier.</t>
   </si>
   <si>
     <t xml:space="preserve">Do you know Scrum already? (1 just heard about it, 5 know it well (process, roles). You are not expected to know Scrum yet, so please be honest. It will not be used for grading what you put here. </t>
-  </si>
-  <si>
-    <t>Preferred team member 1</t>
-  </si>
-  <si>
-    <t>Preferred team member 2</t>
-  </si>
-  <si>
-    <t>Preferred team member 3</t>
-  </si>
-  <si>
-    <t>Preferred team member 4</t>
-  </si>
-  <si>
-    <t>Preferred team member 5</t>
-  </si>
-  <si>
-    <t>Non-preferred student 1</t>
-  </si>
-  <si>
-    <t>Non-preferred student 2</t>
-  </si>
-  <si>
-    <t>Non-preferred student 3</t>
   </si>
   <si>
     <t>2022/10/17 6:31:58 PM EST</t>
@@ -1484,6 +1545,184 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="I5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="I6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="K7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="K8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="K9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1492,105 +1731,105 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="K1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="M1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="N1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="O1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="P1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="Q1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="R1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="S1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="U1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="V1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="W1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="X1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="O2" t="s">
         <v>47</v>
@@ -1599,107 +1838,107 @@
         <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="V2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="W2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="L3" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="P3" t="s">
         <v>46</v>
       </c>
       <c r="Q3" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="R3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="V3" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="W3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="L4" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="M4" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="N4" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="O4" t="s">
         <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="Q4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="V4" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:24">

</xml_diff>

<commit_message>
TSK#201: Finish the update-report command (#85)
</commit_message>
<xml_diff>
--- a/tests/test_files/reports/Example_Report_1.xlsx
+++ b/tests/test_files/reports/Example_Report_1.xlsx
@@ -13,14 +13,15 @@
     <sheet name="individual_report_2" sheetId="4" r:id="rId4"/>
     <sheet name="group_report_2" sheetId="5" r:id="rId5"/>
     <sheet name="overall_report_2" sheetId="6" r:id="rId6"/>
-    <sheet name="survey_data" sheetId="7" r:id="rId7"/>
+    <sheet name="config" sheetId="7" r:id="rId7"/>
+    <sheet name="survey_data" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="127">
   <si>
     <t>Student Id</t>
   </si>
@@ -88,7 +89,7 @@
     <t>monday @ 3:00 AM - 6:00 AM;tuesday @ 3:00 AM - 6:00 AM;wednesday @ 3:00 PM - 6:00 PM;thursday @ 3:00 PM - 6:00 PM;thursday @ 6:00 PM - 9:00 PM;friday @ 9:00 PM - 12:00 PM</t>
   </si>
   <si>
-    <t>jsmith1;bwillia5</t>
+    <t>bwillia5;jsmith1</t>
   </si>
   <si>
     <t>bwillia5</t>
@@ -130,7 +131,7 @@
     <t>Score</t>
   </si>
   <si>
-    <t>mmuster3/jsmith1;mmuster3/bwillia5</t>
+    <t>mmuster3/bwillia5;mmuster3/jsmith1</t>
   </si>
   <si>
     <t>jsmith1/mmuster3</t>
@@ -184,76 +185,136 @@
     <t>7</t>
   </si>
   <si>
+    <t>class_name</t>
+  </si>
+  <si>
+    <t>target_group_size</t>
+  </si>
+  <si>
+    <t>target_plus_one_allowed</t>
+  </si>
+  <si>
+    <t>target_minus_one_allowed</t>
+  </si>
+  <si>
+    <t>grouping_passes</t>
+  </si>
+  <si>
+    <t>availability_values_delimiter</t>
+  </si>
+  <si>
+    <t>student_id_field_name</t>
+  </si>
+  <si>
+    <t>timezone_field_name</t>
+  </si>
+  <si>
+    <t>preferred_students_field_names</t>
+  </si>
+  <si>
+    <t>disliked_students_field_names</t>
+  </si>
+  <si>
+    <t>availability_field_names</t>
+  </si>
+  <si>
+    <t>show_preferred_students</t>
+  </si>
+  <si>
+    <t>show_disliked_students</t>
+  </si>
+  <si>
+    <t>show_availability_overlap</t>
+  </si>
+  <si>
+    <t>show_scores</t>
+  </si>
+  <si>
+    <t>output_student_name</t>
+  </si>
+  <si>
+    <t>output_student_email</t>
+  </si>
+  <si>
+    <t>output_student_login</t>
+  </si>
+  <si>
+    <t>SER401</t>
+  </si>
+  <si>
+    <t>;,</t>
+  </si>
+  <si>
+    <t>Please select your ASURITE ID</t>
+  </si>
+  <si>
+    <t>In what time zone do you live or will you be during the session? Please use UTC so we can match it easier.</t>
+  </si>
+  <si>
+    <t>Preferred team member 1</t>
+  </si>
+  <si>
+    <t>Non-preferred student 1</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [0:00 AM - 3:00 AM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 2</t>
+  </si>
+  <si>
+    <t>Non-preferred student 2</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 AM - 6:00 AM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 3</t>
+  </si>
+  <si>
+    <t>Non-preferred student 3</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 AM - 9:00 AM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 4</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 AM - 12:00 PM]</t>
+  </si>
+  <si>
+    <t>Preferred team member 5</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [12:00 PM - 3:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 PM - 6:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 PM - 9:00 PM]</t>
+  </si>
+  <si>
+    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 PM - 12:00 PM]</t>
+  </si>
+  <si>
     <t>Timestamp</t>
   </si>
   <si>
     <t>Username</t>
   </si>
   <si>
-    <t>Please select your ASURITE ID</t>
-  </si>
-  <si>
     <t>Please enter your Github username (NOT your email address)</t>
   </si>
   <si>
     <t>Email address for us to invite you to the Taiga scrumboard</t>
   </si>
   <si>
-    <t>In what time zone do you live or will you be during the session? Please use UTC so we can match it easier.</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [0:00 AM - 3:00 AM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 AM - 6:00 AM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 AM - 9:00 AM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 AM - 12:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [12:00 PM - 3:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [3:00 PM - 6:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [6:00 PM - 9:00 PM]</t>
-  </si>
-  <si>
-    <t>Please choose times that are good for your team to meet. Times are in the Phoenix, AZ time zone! [9:00 PM - 12:00 PM]</t>
-  </si>
-  <si>
     <t>How well would you say you know GitHub? (1 not at all, 5 worked with it a lot - know how to merge, resolve conflicts, etc.) You are not expected to know GitHub well yet, so please be honest. It will not be used for grading what you put here but I want to try to have one student knowing GitHub in each team to make things easier.</t>
   </si>
   <si>
     <t xml:space="preserve">Do you know Scrum already? (1 just heard about it, 5 know it well (process, roles). You are not expected to know Scrum yet, so please be honest. It will not be used for grading what you put here. </t>
-  </si>
-  <si>
-    <t>Preferred team member 1</t>
-  </si>
-  <si>
-    <t>Preferred team member 2</t>
-  </si>
-  <si>
-    <t>Preferred team member 3</t>
-  </si>
-  <si>
-    <t>Preferred team member 4</t>
-  </si>
-  <si>
-    <t>Preferred team member 5</t>
-  </si>
-  <si>
-    <t>Non-preferred student 1</t>
-  </si>
-  <si>
-    <t>Non-preferred student 2</t>
-  </si>
-  <si>
-    <t>Non-preferred student 3</t>
   </si>
   <si>
     <t>2022/10/17 6:31:58 PM EST</t>
@@ -1484,6 +1545,184 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="I5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="I6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="K7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="K8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="K9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1492,105 +1731,105 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="K1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="M1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="N1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="O1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="P1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="Q1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="R1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="S1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="T1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="U1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="V1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="W1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="X1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="O2" t="s">
         <v>47</v>
@@ -1599,107 +1838,107 @@
         <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="V2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="W2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="L3" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="P3" t="s">
         <v>46</v>
       </c>
       <c r="Q3" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="R3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="V3" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="W3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="L4" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="M4" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="N4" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="O4" t="s">
         <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="Q4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="V4" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:24">

</xml_diff>